<commit_message>
Adding lbw files for 6MW turbine
</commit_message>
<xml_diff>
--- a/examples/H2_Analysis/green_steel_site_renewable_costs.xlsx
+++ b/examples/H2_Analysis/green_steel_site_renewable_costs.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbrunik/github/forked/HOPP/examples/H2_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jannoni/Desktop/HybridPowerPlants/code/green_steel/HOPP/examples/H2_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66FD096D-13C7-C841-BEB8-D07613CA90F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C922BE1A-941D-7D46-861B-1C5717918C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38680" yWindow="9280" windowWidth="27240" windowHeight="15940" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
+    <workbookView xWindow="4320" yWindow="780" windowWidth="33600" windowHeight="19040" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -522,7 +522,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,10 +640,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="3">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C7" s="3">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="D7" s="3">
         <v>225</v>

</xml_diff>

<commit_message>
Added raw materials for steel production costs.
</commit_message>
<xml_diff>
--- a/examples/H2_Analysis/green_steel_site_renewable_costs.xlsx
+++ b/examples/H2_Analysis/green_steel_site_renewable_costs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jannoni/Desktop/HybridPowerPlants/code/green_steel/HOPP/examples/H2_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbrunik/github/forked/HOPP/examples/H2_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C922BE1A-941D-7D46-861B-1C5717918C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539DBAFE-67DC-BD46-B049-4C416432C211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="780" windowWidth="33600" windowHeight="19040" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1FCD4B6C-D650-7B41-B236-554783F4AED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>State</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>30.45, -89.35</t>
+  </si>
+  <si>
+    <t>Lime ($/metric tonne)</t>
+  </si>
+  <si>
+    <t>Carbon ($/metric tonne)</t>
+  </si>
+  <si>
+    <t>Iron Ore Pellets ($/metric tonne)</t>
   </si>
 </sst>
 </file>
@@ -519,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49799FC5-21F5-FB4A-92B9-AD28EDE30D2D}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,6 +957,57 @@
         <v>0.44</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>155.34</v>
+      </c>
+      <c r="C27">
+        <v>141.51</v>
+      </c>
+      <c r="D27">
+        <v>155.34</v>
+      </c>
+      <c r="E27">
+        <v>169.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>218.74</v>
+      </c>
+      <c r="C28">
+        <v>264.94</v>
+      </c>
+      <c r="D28">
+        <v>229.74</v>
+      </c>
+      <c r="E28">
+        <v>245.14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>230.52</v>
+      </c>
+      <c r="C29">
+        <v>292.2</v>
+      </c>
+      <c r="D29">
+        <v>239.32</v>
+      </c>
+      <c r="E29">
+        <v>270.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>